<commit_message>
Unique insertion in family Otididae
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-dependo-side-data.xlsx
+++ b/tabular/eve/epv-dependo-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3C00A0-151C-0047-9725-7C9DA71301FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627E4EC-8104-2C48-BB81-C8AA52ECAD85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="6840" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35184,11 +35184,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7A2856-363C-9149-B6D0-056AF86A7C78}">
   <dimension ref="A1:AF140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R19" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -47233,12 +47236,10 @@
       <c r="B129" t="s">
         <v>1880</v>
       </c>
-      <c r="C129" s="3">
-        <v>0</v>
-      </c>
-      <c r="D129" s="3">
-        <v>1</v>
-      </c>
+      <c r="C129" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" t="s">
         <v>323</v>
@@ -47329,12 +47330,10 @@
       <c r="B130" t="s">
         <v>1880</v>
       </c>
-      <c r="C130" s="3">
-        <v>0</v>
-      </c>
-      <c r="D130" s="3">
-        <v>2</v>
-      </c>
+      <c r="C130" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" t="s">
         <v>323</v>
@@ -47426,11 +47425,9 @@
         <v>1867</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>1970</v>
-      </c>
-      <c r="D131" s="3" t="s">
         <v>1883</v>
       </c>
+      <c r="D131" s="3"/>
       <c r="E131" s="7"/>
       <c r="F131" t="s">
         <v>953</v>
@@ -47522,11 +47519,9 @@
         <v>1867</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>1970</v>
-      </c>
-      <c r="D132" s="3" t="s">
         <v>1883</v>
       </c>
+      <c r="D132" s="3"/>
       <c r="E132" s="7"/>
       <c r="F132" t="s">
         <v>27</v>
@@ -47617,15 +47612,11 @@
       <c r="B133" t="s">
         <v>275</v>
       </c>
-      <c r="C133" s="3">
-        <v>28</v>
-      </c>
-      <c r="D133" s="3">
-        <v>1</v>
-      </c>
-      <c r="E133" s="7" t="s">
-        <v>1996</v>
-      </c>
+      <c r="C133" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D133" s="3"/>
+      <c r="E133" s="7"/>
       <c r="F133" t="s">
         <v>639</v>
       </c>
@@ -47715,15 +47706,11 @@
       <c r="B134" t="s">
         <v>275</v>
       </c>
-      <c r="C134" s="3">
-        <v>28</v>
-      </c>
-      <c r="D134" s="3">
-        <v>1</v>
-      </c>
-      <c r="E134" s="7" t="s">
-        <v>1996</v>
-      </c>
+      <c r="C134" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="7"/>
       <c r="F134" t="s">
         <v>1557</v>
       </c>
@@ -47813,15 +47800,11 @@
       <c r="B135" t="s">
         <v>190</v>
       </c>
-      <c r="C135" s="3">
-        <v>30</v>
-      </c>
-      <c r="D135" s="3">
-        <v>1</v>
-      </c>
-      <c r="E135" s="7" t="s">
-        <v>1997</v>
-      </c>
+      <c r="C135" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D135" s="3"/>
+      <c r="E135" s="7"/>
       <c r="F135" t="s">
         <v>185</v>
       </c>
@@ -47911,15 +47894,11 @@
       <c r="B136" t="s">
         <v>589</v>
       </c>
-      <c r="C136" s="3">
-        <v>157</v>
-      </c>
-      <c r="D136" s="3">
-        <v>1</v>
-      </c>
-      <c r="E136" s="7" t="s">
-        <v>2016</v>
-      </c>
+      <c r="C136" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="7"/>
       <c r="F136" t="s">
         <v>1087</v>
       </c>
@@ -48009,15 +47988,11 @@
       <c r="B137" t="s">
         <v>1221</v>
       </c>
-      <c r="C137" s="3">
-        <v>174</v>
-      </c>
-      <c r="D137" s="3">
-        <v>1</v>
-      </c>
-      <c r="E137" s="7" t="s">
-        <v>2020</v>
-      </c>
+      <c r="C137" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D137" s="3"/>
+      <c r="E137" s="7"/>
       <c r="F137" t="s">
         <v>1215</v>
       </c>
@@ -48107,15 +48082,11 @@
       <c r="B138" t="s">
         <v>1221</v>
       </c>
-      <c r="C138" s="3">
-        <v>174</v>
-      </c>
-      <c r="D138" s="3">
-        <v>1</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>2020</v>
-      </c>
+      <c r="C138" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="7"/>
       <c r="F138" t="s">
         <v>1225</v>
       </c>
@@ -48205,15 +48176,11 @@
       <c r="B139" t="s">
         <v>1974</v>
       </c>
-      <c r="C139" s="3">
-        <v>184</v>
-      </c>
-      <c r="D139" s="3">
-        <v>1</v>
-      </c>
-      <c r="E139" s="7" t="s">
-        <v>2024</v>
-      </c>
+      <c r="C139" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D139" s="3"/>
+      <c r="E139" s="7"/>
       <c r="F139" t="s">
         <v>1087</v>
       </c>
@@ -48303,15 +48270,11 @@
       <c r="B140" t="s">
         <v>292</v>
       </c>
-      <c r="C140" s="3">
-        <v>60</v>
-      </c>
-      <c r="D140" s="3">
-        <v>1</v>
-      </c>
-      <c r="E140" s="7" t="s">
-        <v>2009</v>
-      </c>
+      <c r="C140" s="3" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="7"/>
       <c r="F140" t="s">
         <v>323</v>
       </c>

</xml_diff>